<commit_message>
update data and upload python basic
</commit_message>
<xml_diff>
--- a/data/sample.xlsx
+++ b/data/sample.xlsx
@@ -29,88 +29,88 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
-    <t>이름</t>
+    <t>Kang Daniel</t>
+  </si>
+  <si>
+    <t>Kang Dongho</t>
+  </si>
+  <si>
+    <t>Kang Mina</t>
+  </si>
+  <si>
+    <t>Kwon Hyunbin</t>
+  </si>
+  <si>
+    <t>Kim Doyeon</t>
+  </si>
+  <si>
+    <t>Kim Samuel</t>
+  </si>
+  <si>
+    <t>Kim Sejeong</t>
+  </si>
+  <si>
+    <t>Kim Sohye</t>
+  </si>
+  <si>
+    <t>Kim Chungha</t>
+  </si>
+  <si>
+    <t>Noh Taehyun</t>
+  </si>
+  <si>
+    <t>Lai Kuanlin</t>
+  </si>
+  <si>
+    <t>Park Woojin</t>
+  </si>
+  <si>
+    <t>Park Jihoon</t>
+  </si>
+  <si>
+    <t>Bae Jinyoung</t>
+  </si>
+  <si>
+    <t>Ong Seongwoo</t>
+  </si>
+  <si>
+    <t>Yoo Yeonjung</t>
+  </si>
+  <si>
+    <t>Im Nayoung</t>
+  </si>
+  <si>
+    <t>Jeon Somi</t>
+  </si>
+  <si>
+    <t>Jung Chaeyeon</t>
+  </si>
+  <si>
+    <t>Zhou Jieqiong</t>
+  </si>
+  <si>
+    <t>Ju Haknyeon</t>
+  </si>
+  <si>
+    <t>Choi Yoojung</t>
+  </si>
+  <si>
+    <t>Takada Kenta</t>
+  </si>
+  <si>
+    <t>Ha Sungwoon</t>
+  </si>
+  <si>
+    <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>국어성적</t>
+    <t>Korean</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>수학성적</t>
+    <t>Match</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Kang Daniel</t>
-  </si>
-  <si>
-    <t>Kang Dongho</t>
-  </si>
-  <si>
-    <t>Kang Mina</t>
-  </si>
-  <si>
-    <t>Kwon Hyunbin</t>
-  </si>
-  <si>
-    <t>Kim Doyeon</t>
-  </si>
-  <si>
-    <t>Kim Samuel</t>
-  </si>
-  <si>
-    <t>Kim Sejeong</t>
-  </si>
-  <si>
-    <t>Kim Sohye</t>
-  </si>
-  <si>
-    <t>Kim Chungha</t>
-  </si>
-  <si>
-    <t>Noh Taehyun</t>
-  </si>
-  <si>
-    <t>Lai Kuanlin</t>
-  </si>
-  <si>
-    <t>Park Woojin</t>
-  </si>
-  <si>
-    <t>Park Jihoon</t>
-  </si>
-  <si>
-    <t>Bae Jinyoung</t>
-  </si>
-  <si>
-    <t>Ong Seongwoo</t>
-  </si>
-  <si>
-    <t>Yoo Yeonjung</t>
-  </si>
-  <si>
-    <t>Im Nayoung</t>
-  </si>
-  <si>
-    <t>Jeon Somi</t>
-  </si>
-  <si>
-    <t>Jung Chaeyeon</t>
-  </si>
-  <si>
-    <t>Zhou Jieqiong</t>
-  </si>
-  <si>
-    <t>Ju Haknyeon</t>
-  </si>
-  <si>
-    <t>Choi Yoojung</t>
-  </si>
-  <si>
-    <t>Takada Kenta</t>
-  </si>
-  <si>
-    <t>Ha Sungwoon</t>
   </si>
 </sst>
 </file>
@@ -469,7 +469,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A25"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -479,226 +479,226 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <f ca="1">ROUND(100*RAND(),-1)</f>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2">
         <f ca="1">B2*0.5+50</f>
-        <v>75</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <f t="shared" ref="B3:B24" ca="1" si="0">ROUND(100*RAND(),-1)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:C25" ca="1" si="1">B3*0.5+50</f>
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>65</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>55</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>55</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C10" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="C11" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>95</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="C12" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>50</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C13" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -711,93 +711,93 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="C19" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>80</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="C20" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>80</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B21" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C21" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B22" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="C22" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B23" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C23" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B24" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="C24" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>95</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B25" s="2">
         <f ca="1">ROUND(100*RAND(),-1)</f>
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C25" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>100</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>